<commit_message>
Excel file done, JS buttons WIP
</commit_message>
<xml_diff>
--- a/src/php/output.xlsx
+++ b/src/php/output.xlsx
@@ -113,15 +113,17 @@
     <t>Sales and Retentions</t>
   </si>
   <si>
-    <t>TOTAL</t>
+    <t>TOTALS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
-  <numFmts count="0"/>
-  <fonts count="2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="&quot;£&quot;#,##0.00_-"/>
+  </numFmts>
+  <fonts count="5">
     <font>
       <b val="0"/>
       <i val="0"/>
@@ -140,8 +142,35 @@
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <b val="1"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="11"/>
+      <color rgb="FF0e5373"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="12"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -160,19 +189,128 @@
         <bgColor rgb="FF0e5373"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFdce6f1"/>
+        <bgColor rgb="FFdce6f1"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="13">
     <border/>
     <border>
       <bottom style="medium">
         <color rgb="FFFFFFFF"/>
       </bottom>
     </border>
+    <border>
+      <right style="thin">
+        <color rgb="FF0e5373"/>
+      </right>
+      <bottom style="thin">
+        <color rgb="FF0e5373"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="FF0e5373"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF0e5373"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF0e5373"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="FF0e5373"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF0e5373"/>
+      </top>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF0e5373"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF0e5373"/>
+      </right>
+      <bottom style="thin">
+        <color rgb="FF0e5373"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF0e5373"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF0e5373"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF0e5373"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF0e5373"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF0e5373"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF0e5373"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF0e5373"/>
+      </top>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFFFFFF"/>
+      </right>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF0e5373"/>
+      </left>
+      <bottom style="thin">
+        <color rgb="FF0e5373"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF0e5373"/>
+      </left>
+      <top style="thin">
+        <color rgb="FF0e5373"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF0e5373"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF0e5373"/>
+      </left>
+      <top style="thin">
+        <color rgb="FF0e5373"/>
+      </top>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFFFFFF"/>
+      </left>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="20">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
@@ -185,11 +323,84 @@
     <xf xfId="0" fontId="1" numFmtId="0" fillId="3" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="3" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="4" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0">
+      <alignment vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="4" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0">
+      <alignment vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="4" borderId="4" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0">
+      <alignment vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="4" borderId="5" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0">
+      <alignment vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="4" borderId="6" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0">
+      <alignment vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="4" borderId="7" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0">
+      <alignment vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="4" numFmtId="0" fillId="3" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="164" fillId="4" borderId="5" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="0">
+      <alignment vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="164" fillId="4" borderId="6" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="0">
+      <alignment vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="164" fillId="4" borderId="7" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="0">
+      <alignment vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="4" numFmtId="164" fillId="3" borderId="8" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="164" fillId="4" borderId="9" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="0">
+      <alignment vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="164" fillId="4" borderId="10" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="0">
+      <alignment vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="164" fillId="4" borderId="11" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="0">
+      <alignment vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="4" numFmtId="164" fillId="3" borderId="12" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF008000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFc4d79b"/>
+        </patternFill>
+      </fill>
+      <alignment/>
+      <border/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF800000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFe6b8b7"/>
+        </patternFill>
+      </fill>
+      <alignment/>
+      <border/>
+    </dxf>
+  </dxfs>
   <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
 </styleSheet>
 </file>
@@ -487,7 +698,7 @@
   <dimension ref="A1:Z100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="B2" sqref="B2:G3"/>
+      <selection activeCell="G5" sqref="G5:G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -588,22 +799,22 @@
     </row>
     <row r="4" spans="1:26">
       <c r="A4" s="1"/>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="4" t="s">
         <v>5</v>
       </c>
       <c r="H4" s="1"/>
@@ -628,22 +839,22 @@
     </row>
     <row r="5" spans="1:26">
       <c r="A5" s="1"/>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F5" s="12">
         <v>25000</v>
       </c>
-      <c r="G5" s="1">
+      <c r="G5" s="16">
         <v>21785</v>
       </c>
       <c r="H5" s="1"/>
@@ -668,22 +879,22 @@
     </row>
     <row r="6" spans="1:26">
       <c r="A6" s="1"/>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6" s="13">
         <v>20000</v>
       </c>
-      <c r="G6" s="1">
+      <c r="G6" s="17">
         <v>74321</v>
       </c>
       <c r="H6" s="1"/>
@@ -708,22 +919,22 @@
     </row>
     <row r="7" spans="1:26">
       <c r="A7" s="1"/>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7" s="13">
         <v>20000</v>
       </c>
-      <c r="G7" s="1">
+      <c r="G7" s="17">
         <v>13756</v>
       </c>
       <c r="H7" s="1"/>
@@ -748,22 +959,22 @@
     </row>
     <row r="8" spans="1:26">
       <c r="A8" s="1"/>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F8" s="13">
         <v>20000</v>
       </c>
-      <c r="G8" s="1">
+      <c r="G8" s="17">
         <v>19842</v>
       </c>
       <c r="H8" s="1"/>
@@ -788,22 +999,22 @@
     </row>
     <row r="9" spans="1:26">
       <c r="A9" s="1"/>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F9" s="13">
         <v>20000</v>
       </c>
-      <c r="G9" s="1">
+      <c r="G9" s="17">
         <v>35231</v>
       </c>
       <c r="H9" s="1"/>
@@ -828,22 +1039,22 @@
     </row>
     <row r="10" spans="1:26">
       <c r="A10" s="1"/>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="F10" s="1">
+      <c r="F10" s="13">
         <v>25000</v>
       </c>
-      <c r="G10" s="1">
+      <c r="G10" s="17">
         <v>31983</v>
       </c>
       <c r="H10" s="1"/>
@@ -868,22 +1079,22 @@
     </row>
     <row r="11" spans="1:26">
       <c r="A11" s="1"/>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="F11" s="1">
+      <c r="F11" s="13">
         <v>20000</v>
       </c>
-      <c r="G11" s="1">
+      <c r="G11" s="17">
         <v>25987</v>
       </c>
       <c r="H11" s="1"/>
@@ -908,22 +1119,22 @@
     </row>
     <row r="12" spans="1:26">
       <c r="A12" s="1"/>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="F12" s="1">
+      <c r="F12" s="13">
         <v>20000</v>
       </c>
-      <c r="G12" s="1">
+      <c r="G12" s="17">
         <v>31921</v>
       </c>
       <c r="H12" s="1"/>
@@ -948,22 +1159,22 @@
     </row>
     <row r="13" spans="1:26">
       <c r="A13" s="1"/>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E13" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="F13" s="1">
+      <c r="F13" s="13">
         <v>20000</v>
       </c>
-      <c r="G13" s="1">
+      <c r="G13" s="17">
         <v>45092</v>
       </c>
       <c r="H13" s="1"/>
@@ -988,22 +1199,22 @@
     </row>
     <row r="14" spans="1:26">
       <c r="A14" s="1"/>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E14" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="F14" s="1">
+      <c r="F14" s="14">
         <v>20000</v>
       </c>
-      <c r="G14" s="1">
+      <c r="G14" s="18">
         <v>22543</v>
       </c>
       <c r="H14" s="1"/>
@@ -1028,17 +1239,17 @@
     </row>
     <row r="15" spans="1:26">
       <c r="A15" s="1"/>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1">
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="15">
         <f>SUM(F5:F14)</f>
         <v>210000</v>
       </c>
-      <c r="G15" s="1">
+      <c r="G15" s="19">
         <f>SUM(G5:G14)</f>
         <v>322461</v>
       </c>
@@ -1064,12 +1275,12 @@
     </row>
     <row r="16" spans="1:26">
       <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="19"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
@@ -3446,7 +3657,18 @@
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
   <mergeCells>
     <mergeCell ref="B2:G3"/>
+    <mergeCell ref="B15:E16"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="G15:G16"/>
   </mergeCells>
+  <conditionalFormatting sqref="G5:G14">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+      <formula>25000</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
+      <formula>25000</formula>
+    </cfRule>
+  </conditionalFormatting>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>

</xml_diff>